<commit_message>
Created scatter plots, added areas and latitudes
</commit_message>
<xml_diff>
--- a/datasets/2b - Imports.xlsx
+++ b/datasets/2b - Imports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive\Data analysis projects\Coffee_production_consumption\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7E765D-4B29-47E7-A125-08F23D279975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB5E617-23BE-447B-8848-5CDA657C1415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -237,9 +237,6 @@
     <t>2019</t>
   </si>
   <si>
-    <t xml:space="preserve">   Czechia</t>
-  </si>
-  <si>
     <t>Totals</t>
   </si>
   <si>
@@ -250,6 +247,9 @@
   </si>
   <si>
     <t>Russia</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
   </si>
 </sst>
 </file>
@@ -652,7 +652,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="89" workbookViewId="0">
       <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
       <selection activeCell="A24" sqref="A24"/>
-      <selection pane="topRight" activeCell="A35" sqref="A35"/>
+      <selection pane="topRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -708,7 +708,7 @@
     </row>
     <row r="4" spans="1:32" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -801,7 +801,7 @@
         <v>64</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
@@ -1400,7 +1400,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B11" s="6">
         <v>659.43299999999999</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B34" s="6">
         <v>0</v>
@@ -4069,7 +4069,7 @@
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" s="6">
         <v>21006.786009799998</v>

</xml_diff>